<commit_message>
updated orders (8s after trial 6)
</commit_message>
<xml_diff>
--- a/Experiment/Orders/PAR01_RUN01.xlsx
+++ b/Experiment/Orders/PAR01_RUN01.xlsx
@@ -848,16 +848,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="true"/>
-    <col min="2" max="2" width="15.42578125" customWidth="true"/>
-    <col min="3" max="3" width="17.140625" customWidth="true"/>
-    <col min="4" max="4" width="20.85546875" customWidth="true"/>
-    <col min="5" max="5" width="21" customWidth="true"/>
-    <col min="6" max="6" width="9.85546875" customWidth="true"/>
-    <col min="7" max="7" width="5.85546875" customWidth="true"/>
-    <col min="8" max="8" width="8.7109375" customWidth="true"/>
-    <col min="9" max="9" width="7.140625" customWidth="true"/>
-    <col min="10" max="10" width="5.5703125" customWidth="true"/>
-    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="15.3046875" customWidth="true"/>
+    <col min="3" max="3" width="16.4609375" customWidth="true"/>
+    <col min="4" max="4" width="20.3828125" customWidth="true"/>
+    <col min="5" max="5" width="20.61328125" customWidth="true"/>
+    <col min="6" max="6" width="9.53515625" customWidth="true"/>
+    <col min="7" max="7" width="5.84375" customWidth="true"/>
+    <col min="8" max="8" width="8.4609375" customWidth="true"/>
+    <col min="9" max="9" width="7.15234375" customWidth="true"/>
+    <col min="10" max="10" width="5.765625" customWidth="true"/>
+    <col min="11" max="11" width="11.3046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1358,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>80</v>
@@ -1813,7 +1813,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>87</v>
@@ -2268,7 +2268,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>79</v>
@@ -2723,7 +2723,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>87</v>
@@ -3178,7 +3178,7 @@
         <v>5</v>
       </c>
       <c r="C67" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>80</v>
@@ -3633,7 +3633,7 @@
         <v>5</v>
       </c>
       <c r="C80" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>79</v>
@@ -4088,7 +4088,7 @@
         <v>5</v>
       </c>
       <c r="C93" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>87</v>
@@ -4543,7 +4543,7 @@
         <v>5</v>
       </c>
       <c r="C106" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>79</v>
@@ -4998,7 +4998,7 @@
         <v>5</v>
       </c>
       <c r="C119" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>80</v>
@@ -5453,7 +5453,7 @@
         <v>5</v>
       </c>
       <c r="C132" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>87</v>
@@ -5908,7 +5908,7 @@
         <v>5</v>
       </c>
       <c r="C145" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D145" s="0" t="s">
         <v>80</v>
@@ -6363,7 +6363,7 @@
         <v>5</v>
       </c>
       <c r="C158" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D158" s="0" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
regenerate orders with updates distance/sizes
</commit_message>
<xml_diff>
--- a/Experiment/Orders/PAR01_RUN01.xlsx
+++ b/Experiment/Orders/PAR01_RUN01.xlsx
@@ -27,223 +27,223 @@
     <t>NULL_Change</t>
   </si>
   <si>
-    <t>Face12_D80_S25</t>
+    <t>Face12_D86_S25</t>
   </si>
   <si>
     <t>NULL_ITI</t>
   </si>
   <si>
-    <t>Face03_D80_S30</t>
-  </si>
-  <si>
-    <t>Face09_D80_S30</t>
-  </si>
-  <si>
-    <t>Face16_D80_S25</t>
-  </si>
-  <si>
-    <t>Face05_D80_S20</t>
-  </si>
-  <si>
-    <t>Face07_D80_S20</t>
-  </si>
-  <si>
-    <t>Face02_D51_S30</t>
-  </si>
-  <si>
-    <t>Face15_D51_S30</t>
-  </si>
-  <si>
-    <t>Face14_D51_S25</t>
-  </si>
-  <si>
-    <t>Face18_D51_S20</t>
-  </si>
-  <si>
-    <t>Face04_D51_S20</t>
-  </si>
-  <si>
-    <t>Face13_D51_S25</t>
-  </si>
-  <si>
-    <t>Face06_D64_S30</t>
-  </si>
-  <si>
-    <t>Face08_D64_S25</t>
-  </si>
-  <si>
-    <t>Face11_D64_S20</t>
-  </si>
-  <si>
-    <t>Face01_D64_S30</t>
-  </si>
-  <si>
-    <t>Face17_D64_S20</t>
-  </si>
-  <si>
-    <t>Face10_D64_S25</t>
-  </si>
-  <si>
-    <t>Face16_D51_S25</t>
-  </si>
-  <si>
-    <t>Face12_D51_S20</t>
-  </si>
-  <si>
-    <t>Face05_D51_S30</t>
-  </si>
-  <si>
-    <t>Face10_D51_S20</t>
-  </si>
-  <si>
-    <t>Face02_D51_S25</t>
-  </si>
-  <si>
-    <t>Face13_D51_S30</t>
-  </si>
-  <si>
-    <t>Face15_D80_S25</t>
-  </si>
-  <si>
-    <t>Face01_D80_S25</t>
-  </si>
-  <si>
-    <t>Face08_D80_S30</t>
-  </si>
-  <si>
-    <t>Face18_D80_S30</t>
-  </si>
-  <si>
-    <t>Face11_D80_S20</t>
-  </si>
-  <si>
-    <t>Face03_D80_S20</t>
-  </si>
-  <si>
-    <t>Face04_D64_S25</t>
-  </si>
-  <si>
-    <t>Face09_D64_S30</t>
-  </si>
-  <si>
-    <t>Face07_D64_S20</t>
-  </si>
-  <si>
-    <t>Face06_D64_S20</t>
-  </si>
-  <si>
-    <t>Face14_D64_S25</t>
-  </si>
-  <si>
-    <t>Face17_D64_S30</t>
-  </si>
-  <si>
-    <t>Face16_D51_S20</t>
-  </si>
-  <si>
-    <t>Face01_D51_S20</t>
-  </si>
-  <si>
-    <t>Face07_D51_S30</t>
-  </si>
-  <si>
-    <t>Face14_D51_S30</t>
-  </si>
-  <si>
-    <t>Face15_D51_S25</t>
-  </si>
-  <si>
-    <t>Face06_D51_S25</t>
-  </si>
-  <si>
-    <t>Face18_D64_S20</t>
-  </si>
-  <si>
-    <t>Face08_D64_S30</t>
-  </si>
-  <si>
-    <t>Face10_D64_S30</t>
-  </si>
-  <si>
-    <t>Face03_D64_S25</t>
-  </si>
-  <si>
-    <t>Face11_D64_S25</t>
-  </si>
-  <si>
-    <t>Face09_D64_S20</t>
-  </si>
-  <si>
-    <t>Face04_D80_S20</t>
-  </si>
-  <si>
-    <t>Face17_D80_S25</t>
-  </si>
-  <si>
-    <t>Face02_D80_S30</t>
-  </si>
-  <si>
-    <t>Face12_D80_S20</t>
-  </si>
-  <si>
-    <t>Face13_D80_S30</t>
-  </si>
-  <si>
-    <t>Face05_D80_S25</t>
-  </si>
-  <si>
-    <t>Face03_D51_S20</t>
-  </si>
-  <si>
-    <t>Face08_D51_S30</t>
-  </si>
-  <si>
-    <t>Face02_D51_S20</t>
-  </si>
-  <si>
-    <t>Face09_D51_S25</t>
-  </si>
-  <si>
-    <t>Face01_D51_S25</t>
-  </si>
-  <si>
-    <t>Face16_D51_S30</t>
-  </si>
-  <si>
-    <t>Face15_D80_S30</t>
-  </si>
-  <si>
-    <t>Face18_D80_S20</t>
-  </si>
-  <si>
-    <t>Face06_D80_S25</t>
-  </si>
-  <si>
-    <t>Face04_D80_S25</t>
-  </si>
-  <si>
-    <t>Face14_D80_S20</t>
-  </si>
-  <si>
-    <t>Face05_D80_S30</t>
-  </si>
-  <si>
-    <t>Face12_D64_S20</t>
-  </si>
-  <si>
-    <t>Face10_D64_S20</t>
-  </si>
-  <si>
-    <t>Face07_D64_S25</t>
-  </si>
-  <si>
-    <t>Face17_D64_S25</t>
-  </si>
-  <si>
-    <t>Face11_D64_S30</t>
-  </si>
-  <si>
-    <t>Face13_D64_S30</t>
+    <t>Face03_D86_S31</t>
+  </si>
+  <si>
+    <t>Face09_D86_S31</t>
+  </si>
+  <si>
+    <t>Face16_D86_S25</t>
+  </si>
+  <si>
+    <t>Face05_D86_S20</t>
+  </si>
+  <si>
+    <t>Face07_D86_S20</t>
+  </si>
+  <si>
+    <t>Face02_D55_S31</t>
+  </si>
+  <si>
+    <t>Face15_D55_S31</t>
+  </si>
+  <si>
+    <t>Face14_D55_S25</t>
+  </si>
+  <si>
+    <t>Face18_D55_S20</t>
+  </si>
+  <si>
+    <t>Face04_D55_S20</t>
+  </si>
+  <si>
+    <t>Face13_D55_S25</t>
+  </si>
+  <si>
+    <t>Face06_D69_S31</t>
+  </si>
+  <si>
+    <t>Face08_D69_S25</t>
+  </si>
+  <si>
+    <t>Face11_D69_S20</t>
+  </si>
+  <si>
+    <t>Face01_D69_S31</t>
+  </si>
+  <si>
+    <t>Face17_D69_S20</t>
+  </si>
+  <si>
+    <t>Face10_D69_S25</t>
+  </si>
+  <si>
+    <t>Face16_D55_S25</t>
+  </si>
+  <si>
+    <t>Face12_D55_S20</t>
+  </si>
+  <si>
+    <t>Face05_D55_S31</t>
+  </si>
+  <si>
+    <t>Face10_D55_S20</t>
+  </si>
+  <si>
+    <t>Face02_D55_S25</t>
+  </si>
+  <si>
+    <t>Face13_D55_S31</t>
+  </si>
+  <si>
+    <t>Face15_D86_S25</t>
+  </si>
+  <si>
+    <t>Face01_D86_S25</t>
+  </si>
+  <si>
+    <t>Face08_D86_S31</t>
+  </si>
+  <si>
+    <t>Face18_D86_S31</t>
+  </si>
+  <si>
+    <t>Face11_D86_S20</t>
+  </si>
+  <si>
+    <t>Face03_D86_S20</t>
+  </si>
+  <si>
+    <t>Face04_D69_S25</t>
+  </si>
+  <si>
+    <t>Face09_D69_S31</t>
+  </si>
+  <si>
+    <t>Face07_D69_S20</t>
+  </si>
+  <si>
+    <t>Face06_D69_S20</t>
+  </si>
+  <si>
+    <t>Face14_D69_S25</t>
+  </si>
+  <si>
+    <t>Face17_D69_S31</t>
+  </si>
+  <si>
+    <t>Face16_D55_S20</t>
+  </si>
+  <si>
+    <t>Face01_D55_S20</t>
+  </si>
+  <si>
+    <t>Face07_D55_S31</t>
+  </si>
+  <si>
+    <t>Face14_D55_S31</t>
+  </si>
+  <si>
+    <t>Face15_D55_S25</t>
+  </si>
+  <si>
+    <t>Face06_D55_S25</t>
+  </si>
+  <si>
+    <t>Face18_D69_S20</t>
+  </si>
+  <si>
+    <t>Face08_D69_S31</t>
+  </si>
+  <si>
+    <t>Face10_D69_S31</t>
+  </si>
+  <si>
+    <t>Face03_D69_S25</t>
+  </si>
+  <si>
+    <t>Face11_D69_S25</t>
+  </si>
+  <si>
+    <t>Face09_D69_S20</t>
+  </si>
+  <si>
+    <t>Face04_D86_S20</t>
+  </si>
+  <si>
+    <t>Face17_D86_S25</t>
+  </si>
+  <si>
+    <t>Face02_D86_S31</t>
+  </si>
+  <si>
+    <t>Face12_D86_S20</t>
+  </si>
+  <si>
+    <t>Face13_D86_S31</t>
+  </si>
+  <si>
+    <t>Face05_D86_S25</t>
+  </si>
+  <si>
+    <t>Face03_D55_S20</t>
+  </si>
+  <si>
+    <t>Face08_D55_S31</t>
+  </si>
+  <si>
+    <t>Face02_D55_S20</t>
+  </si>
+  <si>
+    <t>Face09_D55_S25</t>
+  </si>
+  <si>
+    <t>Face01_D55_S25</t>
+  </si>
+  <si>
+    <t>Face16_D55_S31</t>
+  </si>
+  <si>
+    <t>Face15_D86_S31</t>
+  </si>
+  <si>
+    <t>Face18_D86_S20</t>
+  </si>
+  <si>
+    <t>Face06_D86_S25</t>
+  </si>
+  <si>
+    <t>Face04_D86_S25</t>
+  </si>
+  <si>
+    <t>Face14_D86_S20</t>
+  </si>
+  <si>
+    <t>Face05_D86_S31</t>
+  </si>
+  <si>
+    <t>Face12_D69_S20</t>
+  </si>
+  <si>
+    <t>Face10_D69_S20</t>
+  </si>
+  <si>
+    <t>Face07_D69_S25</t>
+  </si>
+  <si>
+    <t>Face17_D69_S25</t>
+  </si>
+  <si>
+    <t>Face11_D69_S31</t>
+  </si>
+  <si>
+    <t>Face13_D69_S31</t>
   </si>
   <si>
     <t>Duration_Seconds</t>
@@ -252,457 +252,457 @@
     <t>Filename_Left</t>
   </si>
   <si>
-    <t>Fixation_D64_l.png</t>
-  </si>
-  <si>
-    <t>Fixation_D80_l.png</t>
-  </si>
-  <si>
-    <t>Face12_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face03_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face09_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face16_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face05_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face07_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Fixation_D51_l.png</t>
-  </si>
-  <si>
-    <t>Face02_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face15_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face14_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face18_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face04_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face13_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face06_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face08_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face11_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face01_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face17_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face10_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face16_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face12_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face05_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face10_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face02_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face13_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face15_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face01_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face08_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face18_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face11_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face03_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face04_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face09_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face07_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face06_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face14_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face17_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face16_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face01_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face07_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face14_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face15_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face06_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face18_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face08_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face10_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face03_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face11_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face09_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face04_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face17_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face02_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face12_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face13_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face05_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face03_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face08_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face02_D51_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face09_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face01_D51_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face16_D51_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face15_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face18_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face06_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face04_D80_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face14_D80_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face05_D80_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face12_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face10_D64_S20_l.png</t>
-  </si>
-  <si>
-    <t>Face07_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face17_D64_S25_l.png</t>
-  </si>
-  <si>
-    <t>Face11_D64_S30_l.png</t>
-  </si>
-  <si>
-    <t>Face13_D64_S30_l.png</t>
+    <t>Fixation_D69_l.png</t>
+  </si>
+  <si>
+    <t>Fixation_D86_l.png</t>
+  </si>
+  <si>
+    <t>Face12_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face03_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face09_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face16_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face05_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face07_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Fixation_D55_l.png</t>
+  </si>
+  <si>
+    <t>Face02_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face15_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face14_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face18_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face04_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face13_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face06_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face08_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face11_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face01_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face17_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face10_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face16_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face12_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face05_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face10_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face02_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face13_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face15_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face01_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face08_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face18_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face11_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face03_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face04_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face09_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face07_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face06_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face14_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face17_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face16_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face01_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face07_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face14_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face15_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face06_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face18_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face08_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face10_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face03_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face11_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face09_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face04_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face17_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face02_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face12_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face13_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face05_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face03_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face08_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face02_D55_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face09_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face01_D55_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face16_D55_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face15_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face18_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face06_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face04_D86_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face14_D86_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face05_D86_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face12_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face10_D69_S20_l.png</t>
+  </si>
+  <si>
+    <t>Face07_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face17_D69_S25_l.png</t>
+  </si>
+  <si>
+    <t>Face11_D69_S31_l.png</t>
+  </si>
+  <si>
+    <t>Face13_D69_S31_l.png</t>
   </si>
   <si>
     <t>Filename_Right</t>
   </si>
   <si>
-    <t>Fixation_D64_r.png</t>
-  </si>
-  <si>
-    <t>Fixation_D80_r.png</t>
-  </si>
-  <si>
-    <t>Face12_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face03_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face09_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face16_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face05_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face07_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Fixation_D51_r.png</t>
-  </si>
-  <si>
-    <t>Face02_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face15_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face14_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face18_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face04_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face13_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face06_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face08_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face11_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face01_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face17_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face10_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face16_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face12_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face05_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face10_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face02_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face13_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face15_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face01_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face08_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face18_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face11_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face03_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face04_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face09_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face07_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face06_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face14_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face17_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face16_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face01_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face07_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face14_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face15_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face06_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face18_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face08_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face10_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face03_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face11_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face09_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face04_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face17_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face02_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face12_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face13_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face05_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face03_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face08_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face02_D51_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face09_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face01_D51_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face16_D51_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face15_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face18_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face06_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face04_D80_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face14_D80_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face05_D80_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face12_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face10_D64_S20_r.png</t>
-  </si>
-  <si>
-    <t>Face07_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face17_D64_S25_r.png</t>
-  </si>
-  <si>
-    <t>Face11_D64_S30_r.png</t>
-  </si>
-  <si>
-    <t>Face13_D64_S30_r.png</t>
+    <t>Fixation_D69_r.png</t>
+  </si>
+  <si>
+    <t>Fixation_D86_r.png</t>
+  </si>
+  <si>
+    <t>Face12_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face03_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face09_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face16_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face05_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face07_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Fixation_D55_r.png</t>
+  </si>
+  <si>
+    <t>Face02_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face15_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face14_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face18_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face04_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face13_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face06_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face08_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face11_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face01_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face17_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face10_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face16_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face12_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face05_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face10_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face02_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face13_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face15_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face01_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face08_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face18_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face11_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face03_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face04_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face09_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face07_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face06_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face14_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face17_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face16_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face01_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face07_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face14_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face15_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face06_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face18_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face08_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face10_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face03_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face11_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face09_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face04_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face17_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face02_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face12_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face13_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face05_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face03_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face08_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face02_D55_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face09_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face01_D55_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face16_D55_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face15_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face18_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face06_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face04_D86_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face14_D86_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face05_D86_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face12_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face10_D69_S20_r.png</t>
+  </si>
+  <si>
+    <t>Face07_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face17_D69_S25_r.png</t>
+  </si>
+  <si>
+    <t>Face11_D69_S31_r.png</t>
+  </si>
+  <si>
+    <t>Face13_D69_S31_r.png</t>
   </si>
   <si>
     <t>Is_Repeat</t>
@@ -714,13 +714,13 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>D64</t>
-  </si>
-  <si>
-    <t>D80</t>
-  </si>
-  <si>
-    <t>D51</t>
+    <t>D69</t>
+  </si>
+  <si>
+    <t>D86</t>
+  </si>
+  <si>
+    <t>D55</t>
   </si>
   <si>
     <t>Face</t>
@@ -789,7 +789,7 @@
     <t>S25</t>
   </si>
   <si>
-    <t>S30</t>
+    <t>S31</t>
   </si>
   <si>
     <t>S20</t>

</xml_diff>